<commit_message>
Adjusting problems with blank and null lines
</commit_message>
<xml_diff>
--- a/lichens/ChecklistofProcessed.xlsx
+++ b/lichens/ChecklistofProcessed.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="171">
   <si>
     <t>NY01075817_lg.txt:     text/plain; charset=utf-8</t>
   </si>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1123,113 +1123,143 @@
       <c r="A26" t="s">
         <v>23</v>
       </c>
+      <c r="E26" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>24</v>
       </c>
+      <c r="E27" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>25</v>
       </c>
+      <c r="E28" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>26</v>
       </c>
+      <c r="E29" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>27</v>
       </c>
+      <c r="E30" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>28</v>
       </c>
+      <c r="E31" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="E32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="E33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="E34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="E35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>45</v>
       </c>

</xml_diff>